<commit_message>
test vs post man
</commit_message>
<xml_diff>
--- a/document/database_batdongsan360.xlsx
+++ b/document/database_batdongsan360.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mydata\University\Nam3Hk2\CongNgheJava\FinalProject\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B936533-E488-4CB1-83EC-4A2703781C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB2D1F5-77B9-4884-9C31-5DDF8640E059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,9 +174,6 @@
     <t>PENDING/SUCCESS/FAILED</t>
   </si>
   <si>
-    <t>POST_SUCCESS/POST_VIEWED/POST_APPROVED/POST_REJECTED/TRANSACTION_SUCCESS/TRANSACTION_FAILED/SYSTEM_ALERT</t>
-  </si>
-  <si>
     <t>PENDING/REVIEW_LATER/APPROVED/REJECTED/EXPIRED</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>ward_id</t>
+  </si>
+  <si>
+    <t>POST/TRANSACTION/SYSTEM_ALERT</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -762,13 +762,13 @@
         <v>4</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -779,7 +779,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>38</v>
@@ -793,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>4</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="G22" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>2</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="G23" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>2</v>
@@ -880,7 +880,7 @@
         <v>30</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>2</v>
@@ -889,7 +889,7 @@
         <v>46</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -900,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>2</v>
@@ -932,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q26" s="4" t="s">
         <v>32</v>
@@ -972,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q28" s="4" t="s">
         <v>2</v>
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>